<commit_message>
把 stcGroupDataAuto 改名为 u32GroupDataAuto
</commit_message>
<xml_diff>
--- a/Flash_Data_Table.xlsx
+++ b/Flash_Data_Table.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="77">
   <si>
     <t>u8GropuNum</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -35,10 +35,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>u16WateringTimeManul</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>u8Channel</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -284,10 +280,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>0xFF, 0xFF</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>0xFF…0xFF</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -305,6 +297,22 @@
   </si>
   <si>
     <t>u8CheckSumBCC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>u8ChannelManual</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>u16WateringTimeManul[0]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>u16WateringTimeManul[1]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0xFF</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -429,7 +437,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -453,6 +461,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -756,10 +767,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:Q6"/>
+  <dimension ref="B2:S6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O28" sqref="O28"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -770,119 +781,130 @@
     <col min="4" max="4" width="12.875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.625" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9" style="1"/>
+    <col min="7" max="7" width="16.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="24.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.625" style="1" customWidth="1"/>
+    <col min="20" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B2" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10"/>
-    </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B3" s="11" t="s">
+    <row r="2" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B2" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="11"/>
+    </row>
+    <row r="3" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B3" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="N3" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="O3" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="P3" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q3" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="R3" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="S3" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="I3" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="J3" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="K3" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="L3" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="M3" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="N3" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="O3" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="P3" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q3" s="11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B4" s="12"/>
+    </row>
+    <row r="4" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B4" s="13"/>
       <c r="C4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="8" t="s">
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="13"/>
+      <c r="P4" s="13"/>
+      <c r="Q4" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="R4" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12"/>
-      <c r="O4" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="P4" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q4" s="12"/>
-    </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="S4" s="13"/>
+    </row>
+    <row r="5" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" s="2">
         <v>8</v>
@@ -896,17 +918,17 @@
       <c r="F5" s="2">
         <v>1</v>
       </c>
-      <c r="G5" s="2">
-        <v>2</v>
+      <c r="G5" s="9">
+        <v>1</v>
       </c>
       <c r="H5" s="2">
+        <v>1</v>
+      </c>
+      <c r="I5" s="2">
         <v>16</v>
       </c>
-      <c r="I5" s="2">
-        <v>8</v>
-      </c>
-      <c r="J5" s="2">
-        <v>8</v>
+      <c r="J5" s="9">
+        <v>16</v>
       </c>
       <c r="K5" s="2">
         <v>8</v>
@@ -915,72 +937,84 @@
         <v>8</v>
       </c>
       <c r="M5" s="2">
+        <v>8</v>
+      </c>
+      <c r="N5" s="2">
+        <v>8</v>
+      </c>
+      <c r="O5" s="2">
         <v>16</v>
       </c>
-      <c r="N5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="O5" s="2">
-        <v>80</v>
-      </c>
-      <c r="P5" s="2">
+      <c r="P5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>64</v>
+      </c>
+      <c r="R5" s="2">
         <v>8</v>
       </c>
-      <c r="Q5" s="2">
+      <c r="S5" s="2">
         <v>408</v>
       </c>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" s="2">
         <v>1</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="10">
         <v>1</v>
       </c>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="2">
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="2">
         <v>2</v>
       </c>
-      <c r="I6" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
-      <c r="M6" s="9"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="2">
-        <v>10</v>
-      </c>
-      <c r="P6" s="2">
+      <c r="J6" s="9">
+        <v>2</v>
+      </c>
+      <c r="K6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="2">
+        <v>8</v>
+      </c>
+      <c r="R6" s="2">
         <v>1</v>
       </c>
-      <c r="Q6" s="2">
+      <c r="S6" s="2">
         <v>51</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="I6:N6"/>
-    <mergeCell ref="B2:Q2"/>
-    <mergeCell ref="Q3:Q4"/>
+  <mergeCells count="17">
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="K6:P6"/>
+    <mergeCell ref="B2:S2"/>
+    <mergeCell ref="S3:S4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
-    <mergeCell ref="H3:H4"/>
     <mergeCell ref="I3:I4"/>
-    <mergeCell ref="J3:J4"/>
     <mergeCell ref="K3:K4"/>
     <mergeCell ref="L3:L4"/>
     <mergeCell ref="M3:M4"/>
     <mergeCell ref="N3:N4"/>
+    <mergeCell ref="O3:O4"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="G3:G4"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1006,90 +1040,90 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B2" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
+      <c r="B2" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="O3" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="I3" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="K3" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="L3" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="M3" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="N3" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="O3" s="14" t="s">
-        <v>30</v>
-      </c>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
       <c r="M4" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="N4" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="N4" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="O4" s="15"/>
+      <c r="O4" s="16"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C5" s="2">
         <v>51</v>
@@ -1169,138 +1203,138 @@
   <sheetData>
     <row r="3" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B9" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B10" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B11" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B12" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B13" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B14" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B15" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B16" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B17" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B18" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B19" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update README.md and resources related.
</commit_message>
<xml_diff>
--- a/Flash_Data_Table.xlsx
+++ b/Flash_Data_Table.xlsx
@@ -296,14 +296,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>u16WateringTimeManul[0]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>u16WateringTimeManul[1]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>0xFF</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -313,6 +305,16 @@
   </si>
   <si>
     <t>enWorkingMode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>u16WateringTimeManual
+[0]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>u16WateringTimeManual
+[1]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -437,7 +439,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -486,6 +488,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -769,8 +774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:S6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6:P6"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -783,7 +788,7 @@
     <col min="6" max="6" width="10.875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="24.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="23.25" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.5" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.375" style="1" bestFit="1" customWidth="1"/>
@@ -826,10 +831,10 @@
         <v>66</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>69</v>
@@ -840,11 +845,11 @@
       <c r="H3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="J3" s="10" t="s">
-        <v>73</v>
+      <c r="I3" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="J3" s="17" t="s">
+        <v>76</v>
       </c>
       <c r="K3" s="10" t="s">
         <v>2</v>
@@ -884,7 +889,7 @@
       <c r="F4" s="11"/>
       <c r="G4" s="11"/>
       <c r="H4" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I4" s="11"/>
       <c r="J4" s="11"/>
@@ -998,6 +1003,7 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="P3:P4"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="J3:J4"/>
     <mergeCell ref="D6:H6"/>
@@ -1014,7 +1020,6 @@
     <mergeCell ref="M3:M4"/>
     <mergeCell ref="N3:N4"/>
     <mergeCell ref="O3:O4"/>
-    <mergeCell ref="P3:P4"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1027,7 +1032,7 @@
   <dimension ref="B2:O5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1191,7 +1196,7 @@
   <dimension ref="A3:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>